<commit_message>
Addition of LJ-Rmin to Class2 and other minor changes
</commit_message>
<xml_diff>
--- a/Atomistic-Class2/WebFF-Class2-DataTemplate.xlsx
+++ b/Atomistic-Class2/WebFF-Class2-DataTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13980" windowHeight="8190" firstSheet="34" activeTab="39"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13980" windowHeight="8190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -35,24 +35,25 @@
     <sheet name="ImproperPotential-Umbrella" sheetId="19" r:id="rId21"/>
     <sheet name="ImproperPotential-CHARMM" sheetId="35" r:id="rId22"/>
     <sheet name="ImproperPotential-Class2" sheetId="40" r:id="rId23"/>
-    <sheet name="NonBondPotential-Class2" sheetId="25" r:id="rId24"/>
-    <sheet name="CrossPotential-BondBond" sheetId="41" r:id="rId25"/>
-    <sheet name="CrossPotential-BondBond13" sheetId="42" r:id="rId26"/>
-    <sheet name="CrossPotential-AngleAngle" sheetId="43" r:id="rId27"/>
-    <sheet name="CrossPotential-BondAngle" sheetId="44" r:id="rId28"/>
-    <sheet name="CrossPotential-MiddleBondTorsio" sheetId="45" r:id="rId29"/>
-    <sheet name="CrossPotential-EndBondTorsion" sheetId="46" r:id="rId30"/>
-    <sheet name="CrossPotential-AngleTorsion" sheetId="47" r:id="rId31"/>
-    <sheet name="CrossPotential-AngleAngleTorsio" sheetId="48" r:id="rId32"/>
-    <sheet name="EquivalenceTable" sheetId="27" r:id="rId33"/>
-    <sheet name="AutoEquivalenceTable" sheetId="33" r:id="rId34"/>
-    <sheet name="BondIncrements" sheetId="28" r:id="rId35"/>
-    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId36"/>
-    <sheet name="AtomType-DFF" sheetId="51" r:id="rId37"/>
-    <sheet name="AtomType-Generic" sheetId="52" r:id="rId38"/>
-    <sheet name="Atom-Attributes-DFF" sheetId="31" r:id="rId39"/>
-    <sheet name="Atom-Attributes-Generic" sheetId="53" r:id="rId40"/>
-    <sheet name="RelationTree-DFF" sheetId="54" r:id="rId41"/>
+    <sheet name="NonBondPotential-LJ-Rmin" sheetId="55" r:id="rId24"/>
+    <sheet name="NonBondPotential-Class2" sheetId="25" r:id="rId25"/>
+    <sheet name="CrossPotential-BondBond" sheetId="41" r:id="rId26"/>
+    <sheet name="CrossPotential-BondBond13" sheetId="42" r:id="rId27"/>
+    <sheet name="CrossPotential-AngleAngle" sheetId="43" r:id="rId28"/>
+    <sheet name="CrossPotential-BondAngle" sheetId="44" r:id="rId29"/>
+    <sheet name="CrossPotential-MiddleBondTorsio" sheetId="45" r:id="rId30"/>
+    <sheet name="CrossPotential-EndBondTorsion" sheetId="46" r:id="rId31"/>
+    <sheet name="CrossPotential-AngleTorsion" sheetId="47" r:id="rId32"/>
+    <sheet name="CrossPotential-AngleAngleTorsio" sheetId="48" r:id="rId33"/>
+    <sheet name="EquivalenceTable" sheetId="27" r:id="rId34"/>
+    <sheet name="AutoEquivalenceTable" sheetId="33" r:id="rId35"/>
+    <sheet name="BondIncrements" sheetId="28" r:id="rId36"/>
+    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId37"/>
+    <sheet name="AtomType-DFF" sheetId="51" r:id="rId38"/>
+    <sheet name="AtomType-Generic" sheetId="52" r:id="rId39"/>
+    <sheet name="Atom-Attributes-DFF" sheetId="31" r:id="rId40"/>
+    <sheet name="Atom-Attributes-Generic" sheetId="53" r:id="rId41"/>
+    <sheet name="RelationTree-DFF" sheetId="54" r:id="rId42"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="306">
   <si>
     <t>Harmonic</t>
   </si>
@@ -305,24 +306,15 @@
     <t>epsilon</t>
   </si>
   <si>
-    <t>sigma</t>
-  </si>
-  <si>
     <t>epsilon-units</t>
   </si>
   <si>
-    <t>sigma-units</t>
-  </si>
-  <si>
     <t>A-units</t>
   </si>
   <si>
     <t>B-units</t>
   </si>
   <si>
-    <t>epsilon*[2*(sigma/R)^9-3*(sigma/R)^6]</t>
-  </si>
-  <si>
     <t>NonBond</t>
   </si>
   <si>
@@ -987,6 +979,21 @@
   </si>
   <si>
     <t>RelationTree</t>
+  </si>
+  <si>
+    <t>Lennard-Jones (12-6) [Rmin Form]</t>
+  </si>
+  <si>
+    <t>epsilon*[(Rmin/R)^12-2*(Rmin/R)^6]</t>
+  </si>
+  <si>
+    <t>Rmin-units</t>
+  </si>
+  <si>
+    <t>Rmin</t>
+  </si>
+  <si>
+    <t>epsilon*[2*(Rmin/R)^9-3*(Rmin/R)^6]</t>
   </si>
 </sst>
 </file>
@@ -1340,7 +1347,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1436,6 +1443,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1450,13 +1467,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1831,10 +1841,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="70"/>
     </row>
     <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -1842,7 +1852,7 @@
     </row>
     <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B3" s="38"/>
     </row>
@@ -1955,7 +1965,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -1967,22 +1977,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -1994,7 +2004,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -2037,13 +2047,13 @@
         <v>30</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2117,7 +2127,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -2129,7 +2139,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>34</v>
@@ -2141,10 +2151,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -2156,7 +2166,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -2187,13 +2197,13 @@
         <v>29</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2252,7 +2262,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>36</v>
@@ -2264,7 +2274,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>37</v>
@@ -2276,10 +2286,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -2291,7 +2301,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -2331,13 +2341,13 @@
         <v>30</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2395,7 +2405,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>43</v>
@@ -2407,7 +2417,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>38</v>
@@ -2419,10 +2429,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -2431,10 +2441,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -2468,13 +2478,13 @@
         <v>42</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2528,10 +2538,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C3" s="5"/>
       <c r="G3" s="5" t="s">
@@ -2540,10 +2550,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5"/>
       <c r="G4" s="5" t="s">
@@ -2552,10 +2562,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="5"/>
       <c r="G5" s="5" t="s">
@@ -2564,10 +2574,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="G6" s="5" t="s">
@@ -2600,16 +2610,16 @@
         <v>42</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J8" s="44" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K8" s="44" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L8" s="44" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2640,7 +2650,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A10:T20"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,7 +2667,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>57</v>
@@ -2669,10 +2679,10 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C4" s="5"/>
       <c r="I4" s="5" t="s">
@@ -2681,10 +2691,10 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="5"/>
       <c r="I5" s="5" t="s">
@@ -2693,10 +2703,10 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="I6" s="5" t="s">
@@ -2705,7 +2715,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -2733,55 +2743,55 @@
         <v>39</v>
       </c>
       <c r="F9" s="45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G9" s="45" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H9" s="45" t="s">
         <v>40</v>
       </c>
       <c r="I9" s="45" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J9" s="45" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K9" s="45" t="s">
         <v>41</v>
       </c>
       <c r="L9" s="45" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M9" s="45" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N9" s="45" t="s">
         <v>42</v>
       </c>
       <c r="O9" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="P9" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q9" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="R9" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="S9" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="P9" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q9" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="R9" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="S9" s="45" t="s">
-        <v>140</v>
-      </c>
       <c r="T9" s="46" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U9" s="46" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V9" s="46" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2837,10 +2847,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C3" s="5"/>
       <c r="F3" s="5" t="s">
@@ -2849,10 +2859,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C4" s="5"/>
       <c r="F4" s="5" t="s">
@@ -2861,10 +2871,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -2873,10 +2883,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -2885,14 +2895,14 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -2920,22 +2930,22 @@
         <v>41</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3006,7 +3016,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>48</v>
@@ -3021,7 +3031,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>49</v>
@@ -3036,10 +3046,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -3054,7 +3064,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -3096,13 +3106,13 @@
         <v>29</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3213,7 +3223,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -3227,7 +3237,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>51</v>
@@ -3241,10 +3251,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -3258,7 +3268,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -3309,13 +3319,13 @@
         <v>54</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3380,7 +3390,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J31" sqref="A10:J31"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,7 +3410,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3412,7 +3422,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>55</v>
@@ -3424,10 +3434,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -3439,7 +3449,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -3479,13 +3489,13 @@
         <v>54</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3531,17 +3541,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="67"/>
+      <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
     </row>
     <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B3" s="12"/>
     </row>
@@ -3554,7 +3564,7 @@
         <v>47</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3611,7 +3621,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>57</v>
@@ -3623,7 +3633,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>61</v>
@@ -3635,10 +3645,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -3650,7 +3660,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -3684,13 +3694,13 @@
         <v>60</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3743,7 +3753,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>62</v>
@@ -3755,7 +3765,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>63</v>
@@ -3767,10 +3777,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="5"/>
       <c r="G5" s="5" t="s">
@@ -3782,7 +3792,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="G6" s="5" t="s">
@@ -3822,13 +3832,13 @@
         <v>64</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3884,7 +3894,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -3896,22 +3906,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -3923,7 +3933,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -3966,13 +3976,13 @@
         <v>30</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4026,10 +4036,10 @@
     <row r="2" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -4038,7 +4048,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>55</v>
@@ -4050,10 +4060,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -4065,7 +4075,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -4105,13 +4115,13 @@
         <v>54</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4145,7 +4155,134 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="A10:I32"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"?,kcal/mol,kJ/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"?,Å,nm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>"epsilon*[(Rmin/R)^12-2*(Rmin/R)^6]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"Lennard-Jones (12-6) [Rmin Form]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>"?,Lorentz-Berthelot,Waldman-Hagler,Kong,Fender-Halsey"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4166,10 +4303,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -4177,10 +4314,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>81</v>
+        <v>305</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -4188,10 +4325,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -4199,10 +4336,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>78</v>
+        <v>303</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -4210,10 +4347,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -4228,16 +4365,16 @@
         <v>75</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>76</v>
+        <v>304</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4249,7 +4386,7 @@
       <formula1>"Lennard-Jones (9-6) [Class 2 Form]"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>"epsilon*[2*(sigma/R)^9-3*(sigma/R)^6]"</formula1>
+      <formula1>"epsilon*[2*(Rmin/R)^9-3*(Rmin/R)^6]"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
       <formula1>"?, kcal/mol, kJ/mol"</formula1>
@@ -4263,7 +4400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -4271,7 +4408,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="A9:I34"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4287,17 +4424,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -4312,10 +4449,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -4329,10 +4466,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -4346,10 +4483,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -4363,10 +4500,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -4400,22 +4537,22 @@
         <v>11</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4440,7 +4577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -4464,18 +4601,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -4491,10 +4628,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -4509,10 +4646,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -4527,10 +4664,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -4545,10 +4682,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -4590,19 +4727,19 @@
         <v>29</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4627,7 +4764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -4652,16 +4789,16 @@
   <sheetData>
     <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C3" s="5"/>
       <c r="H3" s="5" t="s">
@@ -4670,10 +4807,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C4" s="5"/>
       <c r="H4" s="5" t="s">
@@ -4682,10 +4819,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C5" s="5"/>
       <c r="H5" s="5" t="s">
@@ -4694,7 +4831,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -4702,7 +4839,7 @@
       <c r="C6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="51" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4720,31 +4857,31 @@
         <v>28</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4767,7 +4904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -4775,7 +4912,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="A9:I25"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4791,19 +4928,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -4820,10 +4957,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="5"/>
@@ -4839,10 +4976,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="5"/>
@@ -4858,10 +4995,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="5"/>
@@ -4877,10 +5014,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C6" s="52"/>
       <c r="D6" s="5"/>
@@ -4921,25 +5058,25 @@
         <v>15</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4958,203 +5095,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
       <formula1>"BondAngle"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:K8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="A9:I26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="6" width="18" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="36.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="39"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="16"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="16"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
-  </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"MiddleBondTorsion"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>"(R-R2)*[A1*cos(Phi)+A2*cos(2*Phi)+A3*cos(3*Phi)]"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"?, kcal/Å, kJ/nm"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"?, Å, nm"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5168,8 +5108,8 @@
   </sheetPr>
   <dimension ref="A1:A74"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5208,372 +5148,372 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -5586,10 +5526,207 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="6" width="18" customWidth="1"/>
+    <col min="7" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="36.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"MiddleBondTorsion"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>"(R-R2)*[A1*cos(Phi)+A2*cos(2*Phi)+A3*cos(3*Phi)]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"?, kcal/Å, kJ/nm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"?, Å, nm"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="A10:M26"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5605,23 +5742,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -5642,10 +5779,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="5"/>
@@ -5665,10 +5802,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="5"/>
@@ -5688,10 +5825,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="5"/>
@@ -5711,10 +5848,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C6" s="52"/>
       <c r="D6" s="5"/>
@@ -5734,10 +5871,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="5"/>
@@ -5786,13 +5923,13 @@
         <v>28</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H9" s="23" t="s">
         <v>59</v>
@@ -5801,22 +5938,22 @@
         <v>60</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -5841,7 +5978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -5849,7 +5986,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="A10:M30"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5865,23 +6002,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -5902,10 +6039,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="5"/>
@@ -5925,10 +6062,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="5"/>
@@ -5948,10 +6085,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="5"/>
@@ -5971,10 +6108,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C6" s="52"/>
       <c r="D6" s="5"/>
@@ -5982,7 +6119,7 @@
       <c r="F6" s="52"/>
       <c r="G6" s="52"/>
       <c r="H6" s="53" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
@@ -5994,7 +6131,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -6005,7 +6142,7 @@
       <c r="F7" s="52"/>
       <c r="G7" s="52"/>
       <c r="H7" s="53" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
@@ -6046,37 +6183,37 @@
         <v>28</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -6101,7 +6238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -6125,18 +6262,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -6152,10 +6289,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="56"/>
@@ -6170,10 +6307,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="56"/>
@@ -6188,10 +6325,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="56"/>
@@ -6206,7 +6343,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -6214,7 +6351,7 @@
       <c r="C6" s="52"/>
       <c r="D6" s="56"/>
       <c r="E6" s="54" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -6248,22 +6385,22 @@
         <v>28</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -6289,7 +6426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
@@ -6310,32 +6447,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="70"/>
+        <v>86</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="74"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6343,28 +6480,28 @@
         <v>74</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="F5" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>86</v>
-      </c>
       <c r="G5" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -6377,7 +6514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
@@ -6404,40 +6541,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="70"/>
+        <v>86</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="74"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6445,40 +6582,40 @@
         <v>74</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C5" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="23" t="s">
+      <c r="H5" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="I5" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="J5" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="K5" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="L5" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="M5" s="24" t="s">
         <v>124</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -6490,7 +6627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6"/>
@@ -6512,21 +6649,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="41"/>
@@ -6538,25 +6675,25 @@
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>95</v>
-      </c>
       <c r="D5" s="23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -6567,7 +6704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -6591,23 +6728,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -6616,39 +6753,39 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="72" t="s">
-        <v>293</v>
-      </c>
-      <c r="C6" s="72" t="s">
-        <v>294</v>
+        <v>99</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>290</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>291</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6715,7 +6852,134 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O17" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="63"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"?, DFF"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -6739,21 +7003,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -6762,33 +7026,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="72" t="s">
-        <v>296</v>
+        <v>99</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>98</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -6837,7 +7101,7 @@
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"?, DFF"</formula1>
+      <formula1>"?, Generic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6845,129 +7109,158 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
+    <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="43"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>292</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>297</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
+        <v>12</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"?, Generic"</formula1>
+      <formula1>"Harmonic"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>"K*(R-R0)^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"?, kcal/mol/Å^2, kJ/mol/nm^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"?, Å, nm"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6975,7 +7268,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -6984,7 +7277,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7002,7 +7295,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -7010,41 +7303,41 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
+        <v>86</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="24" t="s">
         <v>102</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>298</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -7056,173 +7349,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="A9:G32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="39"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"Harmonic"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>"K*(R-R0)^2"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"?, kcal/mol/Å^2, kJ/mol/nm^2"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"?, Å, nm"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
@@ -7243,7 +7377,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -7251,45 +7385,45 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
+        <v>86</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="24" t="s">
         <v>102</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -7301,7 +7435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -7309,7 +7443,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7320,10 +7454,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
-        <v>302</v>
-      </c>
-      <c r="B1" s="66"/>
+      <c r="A1" s="70" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="70"/>
     </row>
     <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -7331,7 +7465,7 @@
     </row>
     <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B3" s="38"/>
     </row>
@@ -7340,10 +7474,10 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
-        <v>303</v>
-      </c>
-      <c r="B5" s="74"/>
+      <c r="A5" s="68" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7361,7 +7495,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="A9:G27"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7377,17 +7511,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -7402,10 +7536,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C3" s="48"/>
       <c r="D3" s="5"/>
@@ -7419,10 +7553,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="5"/>
@@ -7439,7 +7573,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C5" s="49"/>
       <c r="D5" s="5"/>
@@ -7456,7 +7590,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="5"/>
@@ -7499,13 +7633,13 @@
         <v>7</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -7539,7 +7673,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="A9:G33"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7557,21 +7691,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -7582,7 +7716,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -7596,7 +7730,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -7631,16 +7765,16 @@
         <v>15</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -7693,21 +7827,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -7719,7 +7853,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
@@ -7734,7 +7868,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -7771,16 +7905,16 @@
         <v>15</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -7831,23 +7965,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -7859,7 +7993,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
@@ -7874,7 +8008,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -7898,7 +8032,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -7910,7 +8044,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
@@ -7943,16 +8077,16 @@
         <v>26</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -7992,7 +8126,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="A9:I32"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8010,26 +8144,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -8039,10 +8173,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -8055,7 +8189,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -8100,16 +8234,16 @@
         <v>15</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>